<commit_message>
Updated for Mini Project Part 1
</commit_message>
<xml_diff>
--- a/Computations.xlsx
+++ b/Computations.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukad\Documents\GitHub\Mandelbrot-Mini-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9192F837-7F2B-4478-8C08-947321423DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F6A418-DA06-43F7-B7E0-A6DC5D0827AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77A506D2-D67E-4284-9023-358B7623300F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{77A506D2-D67E-4284-9023-358B7623300F}"/>
   </bookViews>
   <sheets>
     <sheet name="Best Runs" sheetId="6" r:id="rId1"/>
     <sheet name="Optimal chunk size for core" sheetId="7" r:id="rId2"/>
     <sheet name="Core 201 chunk size" sheetId="1" r:id="rId3"/>
-    <sheet name="Core 51 chunk size" sheetId="5" r:id="rId4"/>
-    <sheet name="Chunk Size" sheetId="4" r:id="rId5"/>
+    <sheet name="Chunk Size" sheetId="4" r:id="rId4"/>
+    <sheet name="Core 51 chunk size" sheetId="5" r:id="rId5"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -113,10 +113,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -850,6 +849,7 @@
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
         <c:crossAx val="1779693808"/>
+        <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
         <c:lblOffset val="100"/>
@@ -3068,6 +3068,500 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Chunk Size'!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Average Computation Time Across Cores</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>'Chunk Size'!$D$2:$D$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>191</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>'Chunk Size'!$E$2:$E$161</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="160"/>
+                <c:pt idx="0">
+                  <c:v>1.6493475</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.6024687500000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.5131124999999999</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>1.5148787499999998</c:v>
+                </c:pt>
+                <c:pt idx="32">
+                  <c:v>1.4884962500000001</c:v>
+                </c:pt>
+                <c:pt idx="40">
+                  <c:v>1.5137425</c:v>
+                </c:pt>
+                <c:pt idx="48">
+                  <c:v>1.5002475000000002</c:v>
+                </c:pt>
+                <c:pt idx="56">
+                  <c:v>1.4979987499999998</c:v>
+                </c:pt>
+                <c:pt idx="64">
+                  <c:v>1.4931112499999999</c:v>
+                </c:pt>
+                <c:pt idx="72">
+                  <c:v>1.52549625</c:v>
+                </c:pt>
+                <c:pt idx="80">
+                  <c:v>1.5249787499999998</c:v>
+                </c:pt>
+                <c:pt idx="88">
+                  <c:v>1.5471837499999999</c:v>
+                </c:pt>
+                <c:pt idx="96">
+                  <c:v>1.5167424999999999</c:v>
+                </c:pt>
+                <c:pt idx="104">
+                  <c:v>1.5342349999999998</c:v>
+                </c:pt>
+                <c:pt idx="112">
+                  <c:v>1.57063</c:v>
+                </c:pt>
+                <c:pt idx="120">
+                  <c:v>1.56637125</c:v>
+                </c:pt>
+                <c:pt idx="128">
+                  <c:v>1.5675400000000002</c:v>
+                </c:pt>
+                <c:pt idx="136">
+                  <c:v>1.567075</c:v>
+                </c:pt>
+                <c:pt idx="144">
+                  <c:v>1.5586037500000003</c:v>
+                </c:pt>
+                <c:pt idx="152">
+                  <c:v>1.63860625</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3383-4A7D-850A-C22B932E1BEE}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2050524144"/>
+        <c:axId val="2050527888"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2050524144"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Chunk Size</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2050527888"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2050527888"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Computation Time (s)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2050524144"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:tx>
         <c:rich>
           <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
@@ -4041,501 +4535,6 @@
         </c16r3:dataDisplayOptions16>
       </c:ext>
     </c:extLst>
-    <c:showDLblsOverMax val="0"/>
-  </c:chart>
-  <c:spPr>
-    <a:solidFill>
-      <a:schemeClr val="bg1"/>
-    </a:solidFill>
-    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-      <a:solidFill>
-        <a:schemeClr val="tx1">
-          <a:lumMod val="15000"/>
-          <a:lumOff val="85000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:round/>
-    </a:ln>
-    <a:effectLst/>
-  </c:spPr>
-  <c:txPr>
-    <a:bodyPr/>
-    <a:lstStyle/>
-    <a:p>
-      <a:pPr>
-        <a:defRPr/>
-      </a:pPr>
-      <a:endParaRPr lang="en-DK"/>
-    </a:p>
-  </c:txPr>
-  <c:printSettings>
-    <c:headerFooter/>
-    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
-    <c:pageSetup/>
-  </c:printSettings>
-</c:chartSpace>
-</file>
-
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
-<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
-  <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
-  <c:roundedCorners val="0"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
-      <c14:style val="102"/>
-    </mc:Choice>
-    <mc:Fallback>
-      <c:style val="2"/>
-    </mc:Fallback>
-  </mc:AlternateContent>
-  <c:chart>
-    <c:title>
-      <c:overlay val="0"/>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-      <c:txPr>
-        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-        <a:lstStyle/>
-        <a:p>
-          <a:pPr>
-            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="65000"/>
-                  <a:lumOff val="35000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:latin typeface="+mn-lt"/>
-              <a:ea typeface="+mn-ea"/>
-              <a:cs typeface="+mn-cs"/>
-            </a:defRPr>
-          </a:pPr>
-          <a:endParaRPr lang="en-DK"/>
-        </a:p>
-      </c:txPr>
-    </c:title>
-    <c:autoTitleDeleted val="0"/>
-    <c:plotArea>
-      <c:layout/>
-      <c:barChart>
-        <c:barDir val="col"/>
-        <c:grouping val="clustered"/>
-        <c:varyColors val="0"/>
-        <c:ser>
-          <c:idx val="0"/>
-          <c:order val="0"/>
-          <c:tx>
-            <c:strRef>
-              <c:f>'Chunk Size'!$E$1</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Average Computation Time Across Cores</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
-          </c:tx>
-          <c:spPr>
-            <a:solidFill>
-              <a:schemeClr val="accent1"/>
-            </a:solidFill>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:invertIfNegative val="0"/>
-          <c:cat>
-            <c:numRef>
-              <c:f>'Chunk Size'!$D$2:$D$161</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="160"/>
-                <c:pt idx="0">
-                  <c:v>1</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>11</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>21</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>31</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>41</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>51</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>61</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>71</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>81</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>91</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>101</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>111</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>121</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>131</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>141</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>151</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>161</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>171</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>181</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>191</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:cat>
-          <c:val>
-            <c:numRef>
-              <c:f>'Chunk Size'!$E$2:$E$161</c:f>
-              <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="160"/>
-                <c:pt idx="0">
-                  <c:v>1.6493475</c:v>
-                </c:pt>
-                <c:pt idx="8">
-                  <c:v>1.6024687500000001</c:v>
-                </c:pt>
-                <c:pt idx="16">
-                  <c:v>1.5131124999999999</c:v>
-                </c:pt>
-                <c:pt idx="24">
-                  <c:v>1.5148787499999998</c:v>
-                </c:pt>
-                <c:pt idx="32">
-                  <c:v>1.4884962500000001</c:v>
-                </c:pt>
-                <c:pt idx="40">
-                  <c:v>1.5137425</c:v>
-                </c:pt>
-                <c:pt idx="48">
-                  <c:v>1.5002475000000002</c:v>
-                </c:pt>
-                <c:pt idx="56">
-                  <c:v>1.4979987499999998</c:v>
-                </c:pt>
-                <c:pt idx="64">
-                  <c:v>1.4931112499999999</c:v>
-                </c:pt>
-                <c:pt idx="72">
-                  <c:v>1.52549625</c:v>
-                </c:pt>
-                <c:pt idx="80">
-                  <c:v>1.5249787499999998</c:v>
-                </c:pt>
-                <c:pt idx="88">
-                  <c:v>1.5471837499999999</c:v>
-                </c:pt>
-                <c:pt idx="96">
-                  <c:v>1.5167424999999999</c:v>
-                </c:pt>
-                <c:pt idx="104">
-                  <c:v>1.5342349999999998</c:v>
-                </c:pt>
-                <c:pt idx="112">
-                  <c:v>1.57063</c:v>
-                </c:pt>
-                <c:pt idx="120">
-                  <c:v>1.56637125</c:v>
-                </c:pt>
-                <c:pt idx="128">
-                  <c:v>1.5675400000000002</c:v>
-                </c:pt>
-                <c:pt idx="136">
-                  <c:v>1.567075</c:v>
-                </c:pt>
-                <c:pt idx="144">
-                  <c:v>1.5586037500000003</c:v>
-                </c:pt>
-                <c:pt idx="152">
-                  <c:v>1.63860625</c:v>
-                </c:pt>
-              </c:numCache>
-            </c:numRef>
-          </c:val>
-          <c:extLst>
-            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
-              <c16:uniqueId val="{00000000-3383-4A7D-850A-C22B932E1BEE}"/>
-            </c:ext>
-          </c:extLst>
-        </c:ser>
-        <c:dLbls>
-          <c:dLblPos val="outEnd"/>
-          <c:showLegendKey val="0"/>
-          <c:showVal val="0"/>
-          <c:showCatName val="0"/>
-          <c:showSerName val="0"/>
-          <c:showPercent val="0"/>
-          <c:showBubbleSize val="0"/>
-        </c:dLbls>
-        <c:gapWidth val="219"/>
-        <c:overlap val="-27"/>
-        <c:axId val="2050524144"/>
-        <c:axId val="2050527888"/>
-      </c:barChart>
-      <c:catAx>
-        <c:axId val="2050524144"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="b"/>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="da-DK"/>
-                  <a:t>Chunk Size</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-            <a:solidFill>
-              <a:schemeClr val="tx1">
-                <a:lumMod val="15000"/>
-                <a:lumOff val="85000"/>
-              </a:schemeClr>
-            </a:solidFill>
-            <a:round/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2050527888"/>
-        <c:crosses val="autoZero"/>
-        <c:auto val="1"/>
-        <c:lblAlgn val="ctr"/>
-        <c:lblOffset val="100"/>
-        <c:noMultiLvlLbl val="0"/>
-      </c:catAx>
-      <c:valAx>
-        <c:axId val="2050527888"/>
-        <c:scaling>
-          <c:orientation val="minMax"/>
-        </c:scaling>
-        <c:delete val="0"/>
-        <c:axPos val="l"/>
-        <c:majorGridlines>
-          <c:spPr>
-            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-              <a:solidFill>
-                <a:schemeClr val="tx1">
-                  <a:lumMod val="15000"/>
-                  <a:lumOff val="85000"/>
-                </a:schemeClr>
-              </a:solidFill>
-              <a:round/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-        </c:majorGridlines>
-        <c:title>
-          <c:tx>
-            <c:rich>
-              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-              <a:lstStyle/>
-              <a:p>
-                <a:pPr>
-                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                    <a:solidFill>
-                      <a:schemeClr val="tx1">
-                        <a:lumMod val="65000"/>
-                        <a:lumOff val="35000"/>
-                      </a:schemeClr>
-                    </a:solidFill>
-                    <a:latin typeface="+mn-lt"/>
-                    <a:ea typeface="+mn-ea"/>
-                    <a:cs typeface="+mn-cs"/>
-                  </a:defRPr>
-                </a:pPr>
-                <a:r>
-                  <a:rPr lang="da-DK"/>
-                  <a:t>Computation Time (s)</a:t>
-                </a:r>
-              </a:p>
-            </c:rich>
-          </c:tx>
-          <c:overlay val="0"/>
-          <c:spPr>
-            <a:noFill/>
-            <a:ln>
-              <a:noFill/>
-            </a:ln>
-            <a:effectLst/>
-          </c:spPr>
-          <c:txPr>
-            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-            <a:lstStyle/>
-            <a:p>
-              <a:pPr>
-                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                  <a:solidFill>
-                    <a:schemeClr val="tx1">
-                      <a:lumMod val="65000"/>
-                      <a:lumOff val="35000"/>
-                    </a:schemeClr>
-                  </a:solidFill>
-                  <a:latin typeface="+mn-lt"/>
-                  <a:ea typeface="+mn-ea"/>
-                  <a:cs typeface="+mn-cs"/>
-                </a:defRPr>
-              </a:pPr>
-              <a:endParaRPr lang="en-DK"/>
-            </a:p>
-          </c:txPr>
-        </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
-        <c:majorTickMark val="none"/>
-        <c:minorTickMark val="none"/>
-        <c:tickLblPos val="nextTo"/>
-        <c:spPr>
-          <a:noFill/>
-          <a:ln>
-            <a:noFill/>
-          </a:ln>
-          <a:effectLst/>
-        </c:spPr>
-        <c:txPr>
-          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
-          <a:lstStyle/>
-          <a:p>
-            <a:pPr>
-              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
-                <a:solidFill>
-                  <a:schemeClr val="tx1">
-                    <a:lumMod val="65000"/>
-                    <a:lumOff val="35000"/>
-                  </a:schemeClr>
-                </a:solidFill>
-                <a:latin typeface="+mn-lt"/>
-                <a:ea typeface="+mn-ea"/>
-                <a:cs typeface="+mn-cs"/>
-              </a:defRPr>
-            </a:pPr>
-            <a:endParaRPr lang="en-DK"/>
-          </a:p>
-        </c:txPr>
-        <c:crossAx val="2050524144"/>
-        <c:crosses val="autoZero"/>
-        <c:crossBetween val="between"/>
-      </c:valAx>
-      <c:spPr>
-        <a:noFill/>
-        <a:ln>
-          <a:noFill/>
-        </a:ln>
-        <a:effectLst/>
-      </c:spPr>
-    </c:plotArea>
-    <c:plotVisOnly val="1"/>
-    <c:dispBlanksAs val="gap"/>
     <c:showDLblsOverMax val="0"/>
   </c:chart>
   <c:spPr>
@@ -6294,6 +6293,509 @@
 </file>
 
 <file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -6809,509 +7311,6 @@
 </cs:chartStyle>
 </file>
 
-<file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
-  <cs:axisTitle>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:axisTitle>
-  <cs:categoryAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:categoryAxis>
-  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="bg1"/>
-      </a:solidFill>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="1000" kern="1200"/>
-  </cs:chartArea>
-  <cs:dataLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="75000"/>
-        <a:lumOff val="25000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataLabel>
-  <cs:dataLabelCallout>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln>
-        <a:solidFill>
-          <a:schemeClr val="dk1">
-            <a:lumMod val="25000"/>
-            <a:lumOff val="75000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
-      <a:spAutoFit/>
-    </cs:bodyPr>
-  </cs:dataLabelCallout>
-  <cs:dataPoint>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint>
-  <cs:dataPoint3D>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:dataPoint3D>
-  <cs:dataPointLine>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="28575" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointLine>
-  <cs:dataPointMarker>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1">
-      <cs:styleClr val="auto"/>
-    </cs:fillRef>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointMarker>
-  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
-  <cs:dataPointWireframe>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="1"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dataPointWireframe>
-  <cs:dataTable>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:dataTable>
-  <cs:downBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="dk1">
-          <a:lumMod val="65000"/>
-          <a:lumOff val="35000"/>
-        </a:schemeClr>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:downBar>
-  <cs:dropLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:dropLine>
-  <cs:errorBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="65000"/>
-            <a:lumOff val="35000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:errorBar>
-  <cs:floor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:floor>
-  <cs:gridlineMajor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMajor>
-  <cs:gridlineMinor>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="5000"/>
-            <a:lumOff val="95000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:gridlineMinor>
-  <cs:hiLoLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="75000"/>
-            <a:lumOff val="25000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:hiLoLine>
-  <cs:leaderLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:leaderLine>
-  <cs:legend>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:legend>
-  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea>
-  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-  </cs:plotArea3D>
-  <cs:seriesAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:seriesAxis>
-  <cs:seriesLine>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="35000"/>
-            <a:lumOff val="65000"/>
-          </a:schemeClr>
-        </a:solidFill>
-        <a:round/>
-      </a:ln>
-    </cs:spPr>
-  </cs:seriesLine>
-  <cs:title>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
-  </cs:title>
-  <cs:trendline>
-    <cs:lnRef idx="0">
-      <cs:styleClr val="auto"/>
-    </cs:lnRef>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:ln w="19050" cap="rnd">
-        <a:solidFill>
-          <a:schemeClr val="phClr"/>
-        </a:solidFill>
-        <a:prstDash val="sysDot"/>
-      </a:ln>
-    </cs:spPr>
-  </cs:trendline>
-  <cs:trendlineLabel>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:trendlineLabel>
-  <cs:upBar>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="dk1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="lt1"/>
-      </a:solidFill>
-      <a:ln w="9525">
-        <a:solidFill>
-          <a:schemeClr val="tx1">
-            <a:lumMod val="15000"/>
-            <a:lumOff val="85000"/>
-          </a:schemeClr>
-        </a:solidFill>
-      </a:ln>
-    </cs:spPr>
-  </cs:upBar>
-  <cs:valueAxis>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1">
-        <a:lumMod val="65000"/>
-        <a:lumOff val="35000"/>
-      </a:schemeClr>
-    </cs:fontRef>
-    <cs:defRPr sz="900" kern="1200"/>
-  </cs:valueAxis>
-  <cs:wall>
-    <cs:lnRef idx="0"/>
-    <cs:fillRef idx="0"/>
-    <cs:effectRef idx="0"/>
-    <cs:fontRef idx="minor">
-      <a:schemeClr val="tx1"/>
-    </cs:fontRef>
-    <cs:spPr>
-      <a:noFill/>
-      <a:ln>
-        <a:noFill/>
-      </a:ln>
-    </cs:spPr>
-  </cs:wall>
-</cs:chartStyle>
-</file>
-
 <file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
@@ -7439,6 +7438,47 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>83820</xdr:colOff>
+      <xdr:row>1</xdr:row>
+      <xdr:rowOff>60960</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>16</xdr:col>
+      <xdr:colOff>480060</xdr:colOff>
+      <xdr:row>22</xdr:row>
+      <xdr:rowOff>106680</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E12929DD-3AC4-FBA9-4D53-1E40A7AE9379}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>8</xdr:col>
       <xdr:colOff>596952</xdr:colOff>
       <xdr:row>0</xdr:row>
@@ -7462,47 +7502,6 @@
         <xdr:cNvGraphicFramePr>
           <a:graphicFrameLocks/>
         </xdr:cNvGraphicFramePr>
-      </xdr:nvGraphicFramePr>
-      <xdr:xfrm>
-        <a:off x="0" y="0"/>
-        <a:ext cx="0" cy="0"/>
-      </xdr:xfrm>
-      <a:graphic>
-        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
-          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
-        </a:graphicData>
-      </a:graphic>
-    </xdr:graphicFrame>
-    <xdr:clientData/>
-  </xdr:twoCellAnchor>
-</xdr:wsDr>
-</file>
-
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
-<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
-  <xdr:twoCellAnchor>
-    <xdr:from>
-      <xdr:col>6</xdr:col>
-      <xdr:colOff>83820</xdr:colOff>
-      <xdr:row>1</xdr:row>
-      <xdr:rowOff>60960</xdr:rowOff>
-    </xdr:from>
-    <xdr:to>
-      <xdr:col>16</xdr:col>
-      <xdr:colOff>480060</xdr:colOff>
-      <xdr:row>22</xdr:row>
-      <xdr:rowOff>106680</xdr:rowOff>
-    </xdr:to>
-    <xdr:graphicFrame macro="">
-      <xdr:nvGraphicFramePr>
-        <xdr:cNvPr id="3" name="Chart 2">
-          <a:extLst>
-            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{E12929DD-3AC4-FBA9-4D53-1E40A7AE9379}"/>
-            </a:ext>
-          </a:extLst>
-        </xdr:cNvPr>
-        <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
         <a:off x="0" y="0"/>
@@ -7818,7 +7817,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD862E-865E-4A73-8BE3-21E5FBE40944}">
   <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E11" sqref="E11"/>
     </sheetView>
   </sheetViews>
@@ -9650,10 +9649,10 @@
       <c r="C2" s="1">
         <v>181</v>
       </c>
-      <c r="E2" s="2">
-        <v>1</v>
-      </c>
-      <c r="F2" s="2">
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="F2">
         <f>C2</f>
         <v>181</v>
       </c>
@@ -9668,7 +9667,7 @@
       <c r="C3">
         <v>61</v>
       </c>
-      <c r="E3" s="2">
+      <c r="E3">
         <v>2</v>
       </c>
       <c r="F3">
@@ -9686,7 +9685,7 @@
       <c r="C4">
         <v>41</v>
       </c>
-      <c r="E4" s="2">
+      <c r="E4">
         <v>3</v>
       </c>
       <c r="F4">
@@ -9704,7 +9703,7 @@
       <c r="C5">
         <v>81</v>
       </c>
-      <c r="E5" s="2">
+      <c r="E5">
         <v>4</v>
       </c>
       <c r="F5">
@@ -9722,7 +9721,7 @@
       <c r="C6">
         <v>121</v>
       </c>
-      <c r="E6" s="2">
+      <c r="E6">
         <v>5</v>
       </c>
       <c r="F6">
@@ -9740,7 +9739,7 @@
       <c r="C7">
         <v>21</v>
       </c>
-      <c r="E7" s="2">
+      <c r="E7">
         <v>6</v>
       </c>
       <c r="F7">
@@ -9758,7 +9757,7 @@
       <c r="C8">
         <v>131</v>
       </c>
-      <c r="E8" s="2">
+      <c r="E8">
         <v>7</v>
       </c>
       <c r="F8">
@@ -9776,7 +9775,7 @@
       <c r="C9">
         <v>171</v>
       </c>
-      <c r="E9" s="2">
+      <c r="E9">
         <v>8</v>
       </c>
       <c r="F9">
@@ -14686,989 +14685,10 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D04B6D-C203-4DA7-98F9-CEDA1ABD8977}">
-  <dimension ref="A1:H48"/>
-  <sheetViews>
-    <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="K23" sqref="K23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
-  <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1">
-        <v>2.5765600000000002</v>
-      </c>
-      <c r="D1" t="s">
-        <v>1</v>
-      </c>
-      <c r="E1">
-        <v>1</v>
-      </c>
-      <c r="G1" t="s">
-        <v>2</v>
-      </c>
-      <c r="H1">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A2" t="s">
-        <v>0</v>
-      </c>
-      <c r="B2">
-        <v>2.4770500000000002</v>
-      </c>
-      <c r="D2" t="s">
-        <v>1</v>
-      </c>
-      <c r="E2">
-        <v>1</v>
-      </c>
-      <c r="G2" t="s">
-        <v>2</v>
-      </c>
-      <c r="H2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A3" t="s">
-        <v>0</v>
-      </c>
-      <c r="B3">
-        <v>2.4443899999999998</v>
-      </c>
-      <c r="D3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3">
-        <v>1</v>
-      </c>
-      <c r="G3" t="s">
-        <v>2</v>
-      </c>
-      <c r="H3">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A4" t="s">
-        <v>0</v>
-      </c>
-      <c r="B4">
-        <v>2.46333</v>
-      </c>
-      <c r="D4" t="s">
-        <v>1</v>
-      </c>
-      <c r="E4">
-        <v>1</v>
-      </c>
-      <c r="G4" t="s">
-        <v>2</v>
-      </c>
-      <c r="H4">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A5" t="s">
-        <v>0</v>
-      </c>
-      <c r="B5">
-        <v>2.4402699999999999</v>
-      </c>
-      <c r="D5" t="s">
-        <v>1</v>
-      </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="G5" t="s">
-        <v>2</v>
-      </c>
-      <c r="H5">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A6" t="s">
-        <v>0</v>
-      </c>
-      <c r="B6">
-        <v>2.46007</v>
-      </c>
-      <c r="D6" t="s">
-        <v>1</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="G6" t="s">
-        <v>2</v>
-      </c>
-      <c r="H6">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A7" t="s">
-        <v>0</v>
-      </c>
-      <c r="B7">
-        <v>2.3919899999999998</v>
-      </c>
-      <c r="D7" t="s">
-        <v>1</v>
-      </c>
-      <c r="E7">
-        <v>2</v>
-      </c>
-      <c r="G7" t="s">
-        <v>2</v>
-      </c>
-      <c r="H7">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A8" t="s">
-        <v>0</v>
-      </c>
-      <c r="B8">
-        <v>2.4318900000000001</v>
-      </c>
-      <c r="D8" t="s">
-        <v>1</v>
-      </c>
-      <c r="E8">
-        <v>2</v>
-      </c>
-      <c r="G8" t="s">
-        <v>2</v>
-      </c>
-      <c r="H8">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A9" t="s">
-        <v>0</v>
-      </c>
-      <c r="B9">
-        <v>1.7339899999999999</v>
-      </c>
-      <c r="D9" t="s">
-        <v>1</v>
-      </c>
-      <c r="E9">
-        <v>2</v>
-      </c>
-      <c r="G9" t="s">
-        <v>2</v>
-      </c>
-      <c r="H9">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A10" t="s">
-        <v>0</v>
-      </c>
-      <c r="B10">
-        <v>1.6688700000000001</v>
-      </c>
-      <c r="D10" t="s">
-        <v>1</v>
-      </c>
-      <c r="E10">
-        <v>2</v>
-      </c>
-      <c r="G10" t="s">
-        <v>2</v>
-      </c>
-      <c r="H10">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A11" t="s">
-        <v>0</v>
-      </c>
-      <c r="B11">
-        <v>1.5959700000000001</v>
-      </c>
-      <c r="D11" t="s">
-        <v>1</v>
-      </c>
-      <c r="E11">
-        <v>2</v>
-      </c>
-      <c r="G11" t="s">
-        <v>2</v>
-      </c>
-      <c r="H11">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A12" t="s">
-        <v>0</v>
-      </c>
-      <c r="B12">
-        <v>1.65435</v>
-      </c>
-      <c r="D12" t="s">
-        <v>1</v>
-      </c>
-      <c r="E12">
-        <v>2</v>
-      </c>
-      <c r="G12" t="s">
-        <v>2</v>
-      </c>
-      <c r="H12">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A13" t="s">
-        <v>0</v>
-      </c>
-      <c r="B13">
-        <v>1.4338299999999999</v>
-      </c>
-      <c r="D13" t="s">
-        <v>1</v>
-      </c>
-      <c r="E13">
-        <v>3</v>
-      </c>
-      <c r="G13" t="s">
-        <v>2</v>
-      </c>
-      <c r="H13">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A14" t="s">
-        <v>0</v>
-      </c>
-      <c r="B14">
-        <v>1.2961</v>
-      </c>
-      <c r="D14" t="s">
-        <v>1</v>
-      </c>
-      <c r="E14">
-        <v>3</v>
-      </c>
-      <c r="G14" t="s">
-        <v>2</v>
-      </c>
-      <c r="H14">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A15" t="s">
-        <v>0</v>
-      </c>
-      <c r="B15">
-        <v>1.32107</v>
-      </c>
-      <c r="D15" t="s">
-        <v>1</v>
-      </c>
-      <c r="E15">
-        <v>3</v>
-      </c>
-      <c r="G15" t="s">
-        <v>2</v>
-      </c>
-      <c r="H15">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A16" t="s">
-        <v>0</v>
-      </c>
-      <c r="B16">
-        <v>1.3257300000000001</v>
-      </c>
-      <c r="D16" t="s">
-        <v>1</v>
-      </c>
-      <c r="E16">
-        <v>3</v>
-      </c>
-      <c r="G16" t="s">
-        <v>2</v>
-      </c>
-      <c r="H16">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A17" t="s">
-        <v>0</v>
-      </c>
-      <c r="B17">
-        <v>1.31107</v>
-      </c>
-      <c r="D17" t="s">
-        <v>1</v>
-      </c>
-      <c r="E17">
-        <v>3</v>
-      </c>
-      <c r="G17" t="s">
-        <v>2</v>
-      </c>
-      <c r="H17">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A18" t="s">
-        <v>0</v>
-      </c>
-      <c r="B18">
-        <v>1.3566199999999999</v>
-      </c>
-      <c r="D18" t="s">
-        <v>1</v>
-      </c>
-      <c r="E18">
-        <v>3</v>
-      </c>
-      <c r="G18" t="s">
-        <v>2</v>
-      </c>
-      <c r="H18">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A19" t="s">
-        <v>0</v>
-      </c>
-      <c r="B19">
-        <v>1.32487</v>
-      </c>
-      <c r="D19" t="s">
-        <v>1</v>
-      </c>
-      <c r="E19">
-        <v>4</v>
-      </c>
-      <c r="G19" t="s">
-        <v>2</v>
-      </c>
-      <c r="H19">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A20" t="s">
-        <v>0</v>
-      </c>
-      <c r="B20">
-        <v>1.29182</v>
-      </c>
-      <c r="D20" t="s">
-        <v>1</v>
-      </c>
-      <c r="E20">
-        <v>4</v>
-      </c>
-      <c r="G20" t="s">
-        <v>2</v>
-      </c>
-      <c r="H20">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A21" t="s">
-        <v>0</v>
-      </c>
-      <c r="B21">
-        <v>1.2758799999999999</v>
-      </c>
-      <c r="D21" t="s">
-        <v>1</v>
-      </c>
-      <c r="E21">
-        <v>4</v>
-      </c>
-      <c r="G21" t="s">
-        <v>2</v>
-      </c>
-      <c r="H21">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A22" t="s">
-        <v>0</v>
-      </c>
-      <c r="B22">
-        <v>1.2758400000000001</v>
-      </c>
-      <c r="D22" t="s">
-        <v>1</v>
-      </c>
-      <c r="E22">
-        <v>4</v>
-      </c>
-      <c r="G22" t="s">
-        <v>2</v>
-      </c>
-      <c r="H22">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A23" t="s">
-        <v>0</v>
-      </c>
-      <c r="B23">
-        <v>1.2295</v>
-      </c>
-      <c r="D23" t="s">
-        <v>1</v>
-      </c>
-      <c r="E23">
-        <v>4</v>
-      </c>
-      <c r="G23" t="s">
-        <v>2</v>
-      </c>
-      <c r="H23">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A24" t="s">
-        <v>0</v>
-      </c>
-      <c r="B24">
-        <v>1.2398499999999999</v>
-      </c>
-      <c r="D24" t="s">
-        <v>1</v>
-      </c>
-      <c r="E24">
-        <v>4</v>
-      </c>
-      <c r="G24" t="s">
-        <v>2</v>
-      </c>
-      <c r="H24">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A25" t="s">
-        <v>0</v>
-      </c>
-      <c r="B25">
-        <v>1.3323400000000001</v>
-      </c>
-      <c r="D25" t="s">
-        <v>1</v>
-      </c>
-      <c r="E25">
-        <v>5</v>
-      </c>
-      <c r="G25" t="s">
-        <v>2</v>
-      </c>
-      <c r="H25">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A26" t="s">
-        <v>0</v>
-      </c>
-      <c r="B26">
-        <v>1.28786</v>
-      </c>
-      <c r="D26" t="s">
-        <v>1</v>
-      </c>
-      <c r="E26">
-        <v>5</v>
-      </c>
-      <c r="G26" t="s">
-        <v>2</v>
-      </c>
-      <c r="H26">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A27" t="s">
-        <v>0</v>
-      </c>
-      <c r="B27">
-        <v>1.26936</v>
-      </c>
-      <c r="D27" t="s">
-        <v>1</v>
-      </c>
-      <c r="E27">
-        <v>5</v>
-      </c>
-      <c r="G27" t="s">
-        <v>2</v>
-      </c>
-      <c r="H27">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A28" t="s">
-        <v>0</v>
-      </c>
-      <c r="B28">
-        <v>1.28799</v>
-      </c>
-      <c r="D28" t="s">
-        <v>1</v>
-      </c>
-      <c r="E28">
-        <v>5</v>
-      </c>
-      <c r="G28" t="s">
-        <v>2</v>
-      </c>
-      <c r="H28">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A29" t="s">
-        <v>0</v>
-      </c>
-      <c r="B29">
-        <v>1.28013</v>
-      </c>
-      <c r="D29" t="s">
-        <v>1</v>
-      </c>
-      <c r="E29">
-        <v>5</v>
-      </c>
-      <c r="G29" t="s">
-        <v>2</v>
-      </c>
-      <c r="H29">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A30" t="s">
-        <v>0</v>
-      </c>
-      <c r="B30">
-        <v>1.2623500000000001</v>
-      </c>
-      <c r="D30" t="s">
-        <v>1</v>
-      </c>
-      <c r="E30">
-        <v>5</v>
-      </c>
-      <c r="G30" t="s">
-        <v>2</v>
-      </c>
-      <c r="H30">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A31" t="s">
-        <v>0</v>
-      </c>
-      <c r="B31">
-        <v>1.33474</v>
-      </c>
-      <c r="D31" t="s">
-        <v>1</v>
-      </c>
-      <c r="E31">
-        <v>6</v>
-      </c>
-      <c r="G31" t="s">
-        <v>2</v>
-      </c>
-      <c r="H31">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A32" t="s">
-        <v>0</v>
-      </c>
-      <c r="B32">
-        <v>1.31281</v>
-      </c>
-      <c r="D32" t="s">
-        <v>1</v>
-      </c>
-      <c r="E32">
-        <v>6</v>
-      </c>
-      <c r="G32" t="s">
-        <v>2</v>
-      </c>
-      <c r="H32">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A33" t="s">
-        <v>0</v>
-      </c>
-      <c r="B33">
-        <v>1.2938499999999999</v>
-      </c>
-      <c r="D33" t="s">
-        <v>1</v>
-      </c>
-      <c r="E33">
-        <v>6</v>
-      </c>
-      <c r="G33" t="s">
-        <v>2</v>
-      </c>
-      <c r="H33">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A34" t="s">
-        <v>0</v>
-      </c>
-      <c r="B34">
-        <v>1.3203100000000001</v>
-      </c>
-      <c r="D34" t="s">
-        <v>1</v>
-      </c>
-      <c r="E34">
-        <v>6</v>
-      </c>
-      <c r="G34" t="s">
-        <v>2</v>
-      </c>
-      <c r="H34">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A35" t="s">
-        <v>0</v>
-      </c>
-      <c r="B35">
-        <v>1.3184899999999999</v>
-      </c>
-      <c r="D35" t="s">
-        <v>1</v>
-      </c>
-      <c r="E35">
-        <v>6</v>
-      </c>
-      <c r="G35" t="s">
-        <v>2</v>
-      </c>
-      <c r="H35">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A36" t="s">
-        <v>0</v>
-      </c>
-      <c r="B36">
-        <v>1.3356600000000001</v>
-      </c>
-      <c r="D36" t="s">
-        <v>1</v>
-      </c>
-      <c r="E36">
-        <v>6</v>
-      </c>
-      <c r="G36" t="s">
-        <v>2</v>
-      </c>
-      <c r="H36">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A37" t="s">
-        <v>0</v>
-      </c>
-      <c r="B37">
-        <v>1.3758699999999999</v>
-      </c>
-      <c r="D37" t="s">
-        <v>1</v>
-      </c>
-      <c r="E37">
-        <v>7</v>
-      </c>
-      <c r="G37" t="s">
-        <v>2</v>
-      </c>
-      <c r="H37">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A38" t="s">
-        <v>0</v>
-      </c>
-      <c r="B38">
-        <v>1.31856</v>
-      </c>
-      <c r="D38" t="s">
-        <v>1</v>
-      </c>
-      <c r="E38">
-        <v>7</v>
-      </c>
-      <c r="G38" t="s">
-        <v>2</v>
-      </c>
-      <c r="H38">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A39" t="s">
-        <v>0</v>
-      </c>
-      <c r="B39">
-        <v>1.3449500000000001</v>
-      </c>
-      <c r="D39" t="s">
-        <v>1</v>
-      </c>
-      <c r="E39">
-        <v>7</v>
-      </c>
-      <c r="G39" t="s">
-        <v>2</v>
-      </c>
-      <c r="H39">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A40" t="s">
-        <v>0</v>
-      </c>
-      <c r="B40">
-        <v>1.3536300000000001</v>
-      </c>
-      <c r="D40" t="s">
-        <v>1</v>
-      </c>
-      <c r="E40">
-        <v>7</v>
-      </c>
-      <c r="G40" t="s">
-        <v>2</v>
-      </c>
-      <c r="H40">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A41" t="s">
-        <v>0</v>
-      </c>
-      <c r="B41">
-        <v>1.34419</v>
-      </c>
-      <c r="D41" t="s">
-        <v>1</v>
-      </c>
-      <c r="E41">
-        <v>7</v>
-      </c>
-      <c r="G41" t="s">
-        <v>2</v>
-      </c>
-      <c r="H41">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A42" t="s">
-        <v>0</v>
-      </c>
-      <c r="B42">
-        <v>1.3744400000000001</v>
-      </c>
-      <c r="D42" t="s">
-        <v>1</v>
-      </c>
-      <c r="E42">
-        <v>7</v>
-      </c>
-      <c r="G42" t="s">
-        <v>2</v>
-      </c>
-      <c r="H42">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A43" t="s">
-        <v>0</v>
-      </c>
-      <c r="B43">
-        <v>1.42458</v>
-      </c>
-      <c r="D43" t="s">
-        <v>1</v>
-      </c>
-      <c r="E43">
-        <v>8</v>
-      </c>
-      <c r="G43" t="s">
-        <v>2</v>
-      </c>
-      <c r="H43">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A44" t="s">
-        <v>0</v>
-      </c>
-      <c r="B44">
-        <v>1.4036599999999999</v>
-      </c>
-      <c r="D44" t="s">
-        <v>1</v>
-      </c>
-      <c r="E44">
-        <v>8</v>
-      </c>
-      <c r="G44" t="s">
-        <v>2</v>
-      </c>
-      <c r="H44">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A45" t="s">
-        <v>0</v>
-      </c>
-      <c r="B45">
-        <v>1.4214100000000001</v>
-      </c>
-      <c r="D45" t="s">
-        <v>1</v>
-      </c>
-      <c r="E45">
-        <v>8</v>
-      </c>
-      <c r="G45" t="s">
-        <v>2</v>
-      </c>
-      <c r="H45">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>0</v>
-      </c>
-      <c r="B46">
-        <v>1.42333</v>
-      </c>
-      <c r="D46" t="s">
-        <v>1</v>
-      </c>
-      <c r="E46">
-        <v>8</v>
-      </c>
-      <c r="G46" t="s">
-        <v>2</v>
-      </c>
-      <c r="H46">
-        <v>31</v>
-      </c>
-    </row>
-    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>0</v>
-      </c>
-      <c r="B47">
-        <v>1.38835</v>
-      </c>
-      <c r="D47" t="s">
-        <v>1</v>
-      </c>
-      <c r="E47">
-        <v>8</v>
-      </c>
-      <c r="G47" t="s">
-        <v>2</v>
-      </c>
-      <c r="H47">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
-        <v>0</v>
-      </c>
-      <c r="B48">
-        <v>1.4266000000000001</v>
-      </c>
-      <c r="D48" t="s">
-        <v>1</v>
-      </c>
-      <c r="E48">
-        <v>8</v>
-      </c>
-      <c r="G48" t="s">
-        <v>2</v>
-      </c>
-      <c r="H48">
-        <v>51</v>
-      </c>
-    </row>
-  </sheetData>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H161">
-    <sortCondition ref="E1:E161"/>
-  </sortState>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <drawing r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A99950E-ECAB-4AD6-82DA-4358D4663E12}">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView topLeftCell="B1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -17603,4 +16623,983 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D04B6D-C203-4DA7-98F9-CEDA1ABD8977}">
+  <dimension ref="A1:H48"/>
+  <sheetViews>
+    <sheetView zoomScale="97" workbookViewId="0">
+      <selection activeCell="K23" sqref="K23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1">
+        <v>2.5765600000000002</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1">
+        <v>1</v>
+      </c>
+      <c r="G1" t="s">
+        <v>2</v>
+      </c>
+      <c r="H1">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2">
+        <v>2.4770500000000002</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1</v>
+      </c>
+      <c r="E2">
+        <v>1</v>
+      </c>
+      <c r="G2" t="s">
+        <v>2</v>
+      </c>
+      <c r="H2">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>0</v>
+      </c>
+      <c r="B3">
+        <v>2.4443899999999998</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3">
+        <v>1</v>
+      </c>
+      <c r="G3" t="s">
+        <v>2</v>
+      </c>
+      <c r="H3">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>0</v>
+      </c>
+      <c r="B4">
+        <v>2.46333</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1</v>
+      </c>
+      <c r="E4">
+        <v>1</v>
+      </c>
+      <c r="G4" t="s">
+        <v>2</v>
+      </c>
+      <c r="H4">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>0</v>
+      </c>
+      <c r="B5">
+        <v>2.4402699999999999</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5">
+        <v>1</v>
+      </c>
+      <c r="G5" t="s">
+        <v>2</v>
+      </c>
+      <c r="H5">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>0</v>
+      </c>
+      <c r="B6">
+        <v>2.46007</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1</v>
+      </c>
+      <c r="E6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>2</v>
+      </c>
+      <c r="H6">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>0</v>
+      </c>
+      <c r="B7">
+        <v>2.3919899999999998</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1</v>
+      </c>
+      <c r="E7">
+        <v>2</v>
+      </c>
+      <c r="G7" t="s">
+        <v>2</v>
+      </c>
+      <c r="H7">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>0</v>
+      </c>
+      <c r="B8">
+        <v>2.4318900000000001</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1</v>
+      </c>
+      <c r="E8">
+        <v>2</v>
+      </c>
+      <c r="G8" t="s">
+        <v>2</v>
+      </c>
+      <c r="H8">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>0</v>
+      </c>
+      <c r="B9">
+        <v>1.7339899999999999</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1</v>
+      </c>
+      <c r="E9">
+        <v>2</v>
+      </c>
+      <c r="G9" t="s">
+        <v>2</v>
+      </c>
+      <c r="H9">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>0</v>
+      </c>
+      <c r="B10">
+        <v>1.6688700000000001</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1</v>
+      </c>
+      <c r="E10">
+        <v>2</v>
+      </c>
+      <c r="G10" t="s">
+        <v>2</v>
+      </c>
+      <c r="H10">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>0</v>
+      </c>
+      <c r="B11">
+        <v>1.5959700000000001</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1</v>
+      </c>
+      <c r="E11">
+        <v>2</v>
+      </c>
+      <c r="G11" t="s">
+        <v>2</v>
+      </c>
+      <c r="H11">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>0</v>
+      </c>
+      <c r="B12">
+        <v>1.65435</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1</v>
+      </c>
+      <c r="E12">
+        <v>2</v>
+      </c>
+      <c r="G12" t="s">
+        <v>2</v>
+      </c>
+      <c r="H12">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>0</v>
+      </c>
+      <c r="B13">
+        <v>1.4338299999999999</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1</v>
+      </c>
+      <c r="E13">
+        <v>3</v>
+      </c>
+      <c r="G13" t="s">
+        <v>2</v>
+      </c>
+      <c r="H13">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>0</v>
+      </c>
+      <c r="B14">
+        <v>1.2961</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1</v>
+      </c>
+      <c r="E14">
+        <v>3</v>
+      </c>
+      <c r="G14" t="s">
+        <v>2</v>
+      </c>
+      <c r="H14">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>0</v>
+      </c>
+      <c r="B15">
+        <v>1.32107</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1</v>
+      </c>
+      <c r="E15">
+        <v>3</v>
+      </c>
+      <c r="G15" t="s">
+        <v>2</v>
+      </c>
+      <c r="H15">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>0</v>
+      </c>
+      <c r="B16">
+        <v>1.3257300000000001</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1</v>
+      </c>
+      <c r="E16">
+        <v>3</v>
+      </c>
+      <c r="G16" t="s">
+        <v>2</v>
+      </c>
+      <c r="H16">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>0</v>
+      </c>
+      <c r="B17">
+        <v>1.31107</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1</v>
+      </c>
+      <c r="E17">
+        <v>3</v>
+      </c>
+      <c r="G17" t="s">
+        <v>2</v>
+      </c>
+      <c r="H17">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>0</v>
+      </c>
+      <c r="B18">
+        <v>1.3566199999999999</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1</v>
+      </c>
+      <c r="E18">
+        <v>3</v>
+      </c>
+      <c r="G18" t="s">
+        <v>2</v>
+      </c>
+      <c r="H18">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>0</v>
+      </c>
+      <c r="B19">
+        <v>1.32487</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1</v>
+      </c>
+      <c r="E19">
+        <v>4</v>
+      </c>
+      <c r="G19" t="s">
+        <v>2</v>
+      </c>
+      <c r="H19">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20">
+        <v>1.29182</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1</v>
+      </c>
+      <c r="E20">
+        <v>4</v>
+      </c>
+      <c r="G20" t="s">
+        <v>2</v>
+      </c>
+      <c r="H20">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>0</v>
+      </c>
+      <c r="B21">
+        <v>1.2758799999999999</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1</v>
+      </c>
+      <c r="E21">
+        <v>4</v>
+      </c>
+      <c r="G21" t="s">
+        <v>2</v>
+      </c>
+      <c r="H21">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>0</v>
+      </c>
+      <c r="B22">
+        <v>1.2758400000000001</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1</v>
+      </c>
+      <c r="E22">
+        <v>4</v>
+      </c>
+      <c r="G22" t="s">
+        <v>2</v>
+      </c>
+      <c r="H22">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>0</v>
+      </c>
+      <c r="B23">
+        <v>1.2295</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1</v>
+      </c>
+      <c r="E23">
+        <v>4</v>
+      </c>
+      <c r="G23" t="s">
+        <v>2</v>
+      </c>
+      <c r="H23">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>0</v>
+      </c>
+      <c r="B24">
+        <v>1.2398499999999999</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1</v>
+      </c>
+      <c r="E24">
+        <v>4</v>
+      </c>
+      <c r="G24" t="s">
+        <v>2</v>
+      </c>
+      <c r="H24">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>0</v>
+      </c>
+      <c r="B25">
+        <v>1.3323400000000001</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1</v>
+      </c>
+      <c r="E25">
+        <v>5</v>
+      </c>
+      <c r="G25" t="s">
+        <v>2</v>
+      </c>
+      <c r="H25">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>0</v>
+      </c>
+      <c r="B26">
+        <v>1.28786</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1</v>
+      </c>
+      <c r="E26">
+        <v>5</v>
+      </c>
+      <c r="G26" t="s">
+        <v>2</v>
+      </c>
+      <c r="H26">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>0</v>
+      </c>
+      <c r="B27">
+        <v>1.26936</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1</v>
+      </c>
+      <c r="E27">
+        <v>5</v>
+      </c>
+      <c r="G27" t="s">
+        <v>2</v>
+      </c>
+      <c r="H27">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B28">
+        <v>1.28799</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1</v>
+      </c>
+      <c r="E28">
+        <v>5</v>
+      </c>
+      <c r="G28" t="s">
+        <v>2</v>
+      </c>
+      <c r="H28">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>0</v>
+      </c>
+      <c r="B29">
+        <v>1.28013</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1</v>
+      </c>
+      <c r="E29">
+        <v>5</v>
+      </c>
+      <c r="G29" t="s">
+        <v>2</v>
+      </c>
+      <c r="H29">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>0</v>
+      </c>
+      <c r="B30">
+        <v>1.2623500000000001</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1</v>
+      </c>
+      <c r="E30">
+        <v>5</v>
+      </c>
+      <c r="G30" t="s">
+        <v>2</v>
+      </c>
+      <c r="H30">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>0</v>
+      </c>
+      <c r="B31">
+        <v>1.33474</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1</v>
+      </c>
+      <c r="E31">
+        <v>6</v>
+      </c>
+      <c r="G31" t="s">
+        <v>2</v>
+      </c>
+      <c r="H31">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>0</v>
+      </c>
+      <c r="B32">
+        <v>1.31281</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1</v>
+      </c>
+      <c r="E32">
+        <v>6</v>
+      </c>
+      <c r="G32" t="s">
+        <v>2</v>
+      </c>
+      <c r="H32">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>0</v>
+      </c>
+      <c r="B33">
+        <v>1.2938499999999999</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1</v>
+      </c>
+      <c r="E33">
+        <v>6</v>
+      </c>
+      <c r="G33" t="s">
+        <v>2</v>
+      </c>
+      <c r="H33">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>0</v>
+      </c>
+      <c r="B34">
+        <v>1.3203100000000001</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1</v>
+      </c>
+      <c r="E34">
+        <v>6</v>
+      </c>
+      <c r="G34" t="s">
+        <v>2</v>
+      </c>
+      <c r="H34">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>0</v>
+      </c>
+      <c r="B35">
+        <v>1.3184899999999999</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1</v>
+      </c>
+      <c r="E35">
+        <v>6</v>
+      </c>
+      <c r="G35" t="s">
+        <v>2</v>
+      </c>
+      <c r="H35">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>0</v>
+      </c>
+      <c r="B36">
+        <v>1.3356600000000001</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1</v>
+      </c>
+      <c r="E36">
+        <v>6</v>
+      </c>
+      <c r="G36" t="s">
+        <v>2</v>
+      </c>
+      <c r="H36">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>0</v>
+      </c>
+      <c r="B37">
+        <v>1.3758699999999999</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1</v>
+      </c>
+      <c r="E37">
+        <v>7</v>
+      </c>
+      <c r="G37" t="s">
+        <v>2</v>
+      </c>
+      <c r="H37">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>0</v>
+      </c>
+      <c r="B38">
+        <v>1.31856</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1</v>
+      </c>
+      <c r="E38">
+        <v>7</v>
+      </c>
+      <c r="G38" t="s">
+        <v>2</v>
+      </c>
+      <c r="H38">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>0</v>
+      </c>
+      <c r="B39">
+        <v>1.3449500000000001</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1</v>
+      </c>
+      <c r="E39">
+        <v>7</v>
+      </c>
+      <c r="G39" t="s">
+        <v>2</v>
+      </c>
+      <c r="H39">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>0</v>
+      </c>
+      <c r="B40">
+        <v>1.3536300000000001</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1</v>
+      </c>
+      <c r="E40">
+        <v>7</v>
+      </c>
+      <c r="G40" t="s">
+        <v>2</v>
+      </c>
+      <c r="H40">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>0</v>
+      </c>
+      <c r="B41">
+        <v>1.34419</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1</v>
+      </c>
+      <c r="E41">
+        <v>7</v>
+      </c>
+      <c r="G41" t="s">
+        <v>2</v>
+      </c>
+      <c r="H41">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>0</v>
+      </c>
+      <c r="B42">
+        <v>1.3744400000000001</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1</v>
+      </c>
+      <c r="E42">
+        <v>7</v>
+      </c>
+      <c r="G42" t="s">
+        <v>2</v>
+      </c>
+      <c r="H42">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>0</v>
+      </c>
+      <c r="B43">
+        <v>1.42458</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1</v>
+      </c>
+      <c r="E43">
+        <v>8</v>
+      </c>
+      <c r="G43" t="s">
+        <v>2</v>
+      </c>
+      <c r="H43">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>0</v>
+      </c>
+      <c r="B44">
+        <v>1.4036599999999999</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1</v>
+      </c>
+      <c r="E44">
+        <v>8</v>
+      </c>
+      <c r="G44" t="s">
+        <v>2</v>
+      </c>
+      <c r="H44">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>0</v>
+      </c>
+      <c r="B45">
+        <v>1.4214100000000001</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1</v>
+      </c>
+      <c r="E45">
+        <v>8</v>
+      </c>
+      <c r="G45" t="s">
+        <v>2</v>
+      </c>
+      <c r="H45">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>0</v>
+      </c>
+      <c r="B46">
+        <v>1.42333</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1</v>
+      </c>
+      <c r="E46">
+        <v>8</v>
+      </c>
+      <c r="G46" t="s">
+        <v>2</v>
+      </c>
+      <c r="H46">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>0</v>
+      </c>
+      <c r="B47">
+        <v>1.38835</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1</v>
+      </c>
+      <c r="E47">
+        <v>8</v>
+      </c>
+      <c r="G47" t="s">
+        <v>2</v>
+      </c>
+      <c r="H47">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>0</v>
+      </c>
+      <c r="B48">
+        <v>1.4266000000000001</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1</v>
+      </c>
+      <c r="E48">
+        <v>8</v>
+      </c>
+      <c r="G48" t="s">
+        <v>2</v>
+      </c>
+      <c r="H48">
+        <v>51</v>
+      </c>
+    </row>
+  </sheetData>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A1:H161">
+    <sortCondition ref="E1:E161"/>
+  </sortState>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
Final Part 1 submit for Mini Project
</commit_message>
<xml_diff>
--- a/Computations.xlsx
+++ b/Computations.xlsx
@@ -8,16 +8,17 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lukad\Documents\GitHub\Mandelbrot-Mini-Project\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A4F6A418-DA06-43F7-B7E0-A6DC5D0827AC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{ABF7A3FE-48AC-49ED-AE34-25320C5037F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{77A506D2-D67E-4284-9023-358B7623300F}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{77A506D2-D67E-4284-9023-358B7623300F}"/>
   </bookViews>
   <sheets>
     <sheet name="Best Runs" sheetId="6" r:id="rId1"/>
-    <sheet name="Optimal chunk size for core" sheetId="7" r:id="rId2"/>
-    <sheet name="Core 201 chunk size" sheetId="1" r:id="rId3"/>
-    <sheet name="Chunk Size" sheetId="4" r:id="rId4"/>
-    <sheet name="Core 51 chunk size" sheetId="5" r:id="rId5"/>
+    <sheet name="Speedup" sheetId="8" r:id="rId2"/>
+    <sheet name="Optimal chunk size for core" sheetId="7" r:id="rId3"/>
+    <sheet name="Core 201 chunk size" sheetId="1" r:id="rId4"/>
+    <sheet name="Chunk Size" sheetId="4" r:id="rId5"/>
+    <sheet name="Core 51 chunk size" sheetId="5" r:id="rId6"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="637" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="645" uniqueCount="15">
   <si>
     <t>time:</t>
   </si>
@@ -71,11 +72,29 @@
   <si>
     <t>Chunk Size (optimal)</t>
   </si>
+  <si>
+    <t>Speedup</t>
+  </si>
+  <si>
+    <t>Efficiency</t>
+  </si>
+  <si>
+    <t>Overhead</t>
+  </si>
+  <si>
+    <t>Chunksize</t>
+  </si>
+  <si>
+    <t>Computation Time(s)</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <numFmts count="1">
+    <numFmt numFmtId="164" formatCode="0.000"/>
+  </numFmts>
   <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -113,9 +132,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -946,6 +967,1599 @@
   </mc:AlternateContent>
   <c:chart>
     <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="da-DK"/>
+              <a:t>Speedup,</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="da-DK" baseline="0"/>
+              <a:t> Efficiency and Overhead across cores</a:t>
+            </a:r>
+            <a:endParaRPr lang="da-DK"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:barChart>
+        <c:barDir val="col"/>
+        <c:grouping val="clustered"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedup!$B$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Computation Time (s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent1"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Speedup!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Speedup!$B$2:$B$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>2.4390200000000002</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5643800000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.3364400000000001</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2412000000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2811399999999999</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.3154300000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.34063</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.4343300000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-1E8E-47EA-9CFA-CDB2C6A01120}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedup!$C$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent2"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Speedup!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Speedup!$C$2:$C$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.5590968946163977</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.8250127203615576</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.9650499516596842</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.9037888130883434</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.8541617569920101</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.8193088324146112</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.7004594479652522</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-1E8E-47EA-9CFA-CDB2C6A01120}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedup!$D$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Efficiency</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent3"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Speedup!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Speedup!$D$2:$D$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.77954844730819883</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.60833757345385253</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>0.49126248791492105</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.38075776261766869</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.30902695949866837</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.25990126177351586</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.21255743099565652</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-1E8E-47EA-9CFA-CDB2C6A01120}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="3"/>
+          <c:order val="3"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedup!$E$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Overhead</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:solidFill>
+              <a:schemeClr val="accent4"/>
+            </a:solidFill>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:invertIfNegative val="0"/>
+          <c:cat>
+            <c:numRef>
+              <c:f>Speedup!$A$2:$A$9</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Speedup!$E$2:$E$9</c:f>
+              <c:numCache>
+                <c:formatCode>0.000</c:formatCode>
+                <c:ptCount val="8"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.68974000000000002</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.5703000000000005</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>2.5257800000000001</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>3.9666799999999993</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.4535600000000004</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.9453899999999988</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>9.0356200000000015</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000003-1E8E-47EA-9CFA-CDB2C6A01120}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:gapWidth val="219"/>
+        <c:overlap val="-27"/>
+        <c:axId val="2088378959"/>
+        <c:axId val="2088380623"/>
+      </c:barChart>
+      <c:catAx>
+        <c:axId val="2088378959"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Number</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="da-DK" baseline="0"/>
+                  <a:t> of cores</a:t>
+                </a:r>
+                <a:endParaRPr lang="da-DK"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2088380623"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="2088380623"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Result</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.000" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="2088378959"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="da-DK"/>
+              <a:t>Speedup for chunksize</a:t>
+            </a:r>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:lineChart>
+        <c:grouping val="standard"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedup!$K$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Computation Time(s)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Speedup!$J$2:$J$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Speedup!$K$2:$K$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1.3895999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3033600000000001</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.36557</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.2412099999999999</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.2907500000000001</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.22899</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.2160500000000001</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.28942</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.2352000000000001</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.23133</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.28267</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.3347800000000001</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.2574399999999999</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.2799799999999999</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>1.44651</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>1.4887900000000001</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.3243</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.34728</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.35225</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>1.43207</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>1.40455</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-352F-4202-96CE-0FB9E0923BD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>Speedup!$L$1</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Speedup</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent2"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:cat>
+            <c:numRef>
+              <c:f>Speedup!$J$2:$J$22</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>31</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>41</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>51</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>61</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>71</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>81</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>91</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>101</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>111</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>121</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>131</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>141</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>151</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>161</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>171</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>181</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>191</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>201</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:cat>
+          <c:val>
+            <c:numRef>
+              <c:f>Speedup!$L$2:$L$22</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="21"/>
+                <c:pt idx="0">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0661674441443652</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>1.0175970473868055</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>1.1195526945480621</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>1.0765833817547936</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>1.1306845458465895</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>1.1427161712100653</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>1.0776938468458686</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1.1249999999999998</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>1.1285358108711718</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>1.0833651679699376</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>1.0410704385741469</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>1.1051024303346482</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>1.0856419631556744</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>0.96065702967832922</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>0.93337542568125786</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>1.0493090689420825</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>1.031411436375512</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>1.027620632279534</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>0.97034362845391631</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>0.98935602150154855</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:val>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-352F-4202-96CE-0FB9E0923BD4}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:smooth val="0"/>
+        <c:axId val="654909328"/>
+        <c:axId val="654909744"/>
+      </c:lineChart>
+      <c:catAx>
+        <c:axId val="654909328"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Chunk</a:t>
+                </a:r>
+                <a:r>
+                  <a:rPr lang="da-DK" baseline="0"/>
+                  <a:t> Size</a:t>
+                </a:r>
+                <a:endParaRPr lang="da-DK"/>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654909744"/>
+        <c:crosses val="autoZero"/>
+        <c:auto val="1"/>
+        <c:lblAlgn val="ctr"/>
+        <c:lblOffset val="100"/>
+        <c:noMultiLvlLbl val="0"/>
+      </c:catAx>
+      <c:valAx>
+        <c:axId val="654909744"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="da-DK"/>
+                  <a:t>Result</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-DK"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln>
+            <a:noFill/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="654909328"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="between"/>
+      </c:valAx>
+      <c:dTable>
+        <c:showHorzBorder val="1"/>
+        <c:showVertBorder val="1"/>
+        <c:showOutline val="1"/>
+        <c:showKeys val="1"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="15000"/>
+                <a:lumOff val="85000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr rtl="0">
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-DK"/>
+          </a:p>
+        </c:txPr>
+      </c:dTable>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="b"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-DK"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-DK"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
       <c:overlay val="0"/>
       <c:spPr>
         <a:noFill/>
@@ -1353,7 +2967,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3053,7 +4667,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -3547,7 +5161,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
   <c:lang val="en-US"/>
@@ -4770,6 +6384,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors7.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
@@ -5777,7 +7471,7 @@
 </file>
 
 <file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
-<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
     <cs:fillRef idx="0"/>
@@ -5885,11 +7579,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint>
   <cs:dataPoint3D>
     <cs:lnRef idx="0"/>
@@ -5900,11 +7589,6 @@
     <cs:fontRef idx="minor">
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
-    <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
-    </cs:spPr>
   </cs:dataPoint3D>
   <cs:dataPointLine>
     <cs:lnRef idx="0">
@@ -5936,9 +7620,6 @@
       <a:schemeClr val="tx1"/>
     </cs:fontRef>
     <cs:spPr>
-      <a:solidFill>
-        <a:schemeClr val="phClr"/>
-      </a:solidFill>
       <a:ln w="9525">
         <a:solidFill>
           <a:schemeClr val="phClr"/>
@@ -6796,6 +8477,1025 @@
 </file>
 
 <file path=xl/charts/style5.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+    </cs:spPr>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="phClr"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style6.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="201">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="28575" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="65000"/>
+          <a:lumOff val="35000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="75000"/>
+            <a:lumOff val="25000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style7.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="227">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -7356,6 +10056,83 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
+      <xdr:col>0</xdr:col>
+      <xdr:colOff>281940</xdr:colOff>
+      <xdr:row>10</xdr:row>
+      <xdr:rowOff>7620</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>7</xdr:col>
+      <xdr:colOff>411480</xdr:colOff>
+      <xdr:row>35</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{F0C9827E-57CA-777F-3B2A-691F69EBC7FF}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>12</xdr:col>
+      <xdr:colOff>548640</xdr:colOff>
+      <xdr:row>3</xdr:row>
+      <xdr:rowOff>137160</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>25</xdr:col>
+      <xdr:colOff>91440</xdr:colOff>
+      <xdr:row>27</xdr:row>
+      <xdr:rowOff>45720</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4B2FC753-AD25-189C-4A28-BA87AEECA3E2}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
       <xdr:col>6</xdr:col>
       <xdr:colOff>601980</xdr:colOff>
       <xdr:row>1</xdr:row>
@@ -7393,7 +10170,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7434,7 +10211,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7475,7 +10252,7 @@
 </xdr:wsDr>
 </file>
 
-<file path=xl/drawings/drawing5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/drawings/drawing6.xml><?xml version="1.0" encoding="utf-8"?>
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:twoCellAnchor>
     <xdr:from>
@@ -7817,8 +10594,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E0FD862E-865E-4A73-8BE3-21E5FBE40944}">
   <dimension ref="A1:C161"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E3" sqref="E3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -9608,6 +12385,495 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{380D8475-F855-4112-BA04-E6D740354F4F}">
+  <dimension ref="A1:N22"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I5" sqref="I5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="8.33203125" customWidth="1"/>
+    <col min="2" max="2" width="18.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="16.109375" customWidth="1"/>
+    <col min="4" max="4" width="13.6640625" customWidth="1"/>
+    <col min="5" max="5" width="15" customWidth="1"/>
+    <col min="11" max="11" width="18.21875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>5</v>
+      </c>
+      <c r="C1" t="s">
+        <v>10</v>
+      </c>
+      <c r="D1" t="s">
+        <v>11</v>
+      </c>
+      <c r="E1" t="s">
+        <v>12</v>
+      </c>
+      <c r="J1" t="s">
+        <v>13</v>
+      </c>
+      <c r="K1" t="s">
+        <v>14</v>
+      </c>
+      <c r="L1" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="2" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A2">
+        <v>1</v>
+      </c>
+      <c r="B2" s="2">
+        <v>2.4390200000000002</v>
+      </c>
+      <c r="C2" s="2">
+        <f>B$2/B2</f>
+        <v>1</v>
+      </c>
+      <c r="D2" s="2">
+        <f>C2/A2</f>
+        <v>1</v>
+      </c>
+      <c r="E2" s="2">
+        <f>A2*B2-B$2</f>
+        <v>0</v>
+      </c>
+      <c r="J2">
+        <v>1</v>
+      </c>
+      <c r="K2" s="3">
+        <v>1.3895999999999999</v>
+      </c>
+      <c r="L2" s="3">
+        <f>K$2/K2</f>
+        <v>1</v>
+      </c>
+      <c r="M2" s="2"/>
+      <c r="N2" s="2"/>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A3">
+        <v>2</v>
+      </c>
+      <c r="B3" s="2">
+        <v>1.5643800000000001</v>
+      </c>
+      <c r="C3" s="2">
+        <f>B$2/B3</f>
+        <v>1.5590968946163977</v>
+      </c>
+      <c r="D3" s="2">
+        <f t="shared" ref="D3:D9" si="0">C3/A3</f>
+        <v>0.77954844730819883</v>
+      </c>
+      <c r="E3" s="2">
+        <f t="shared" ref="E3:E9" si="1">A3*B3-B$2</f>
+        <v>0.68974000000000002</v>
+      </c>
+      <c r="J3">
+        <v>11</v>
+      </c>
+      <c r="K3" s="3">
+        <v>1.3033600000000001</v>
+      </c>
+      <c r="L3" s="3">
+        <f>K$2/K3</f>
+        <v>1.0661674441443652</v>
+      </c>
+      <c r="M3" s="2"/>
+      <c r="N3" s="2"/>
+    </row>
+    <row r="4" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A4">
+        <v>3</v>
+      </c>
+      <c r="B4" s="2">
+        <v>1.3364400000000001</v>
+      </c>
+      <c r="C4" s="2">
+        <f t="shared" ref="C4:C9" si="2">B$2/B4</f>
+        <v>1.8250127203615576</v>
+      </c>
+      <c r="D4" s="2">
+        <f t="shared" si="0"/>
+        <v>0.60833757345385253</v>
+      </c>
+      <c r="E4" s="2">
+        <f t="shared" si="1"/>
+        <v>1.5703000000000005</v>
+      </c>
+      <c r="J4">
+        <v>21</v>
+      </c>
+      <c r="K4" s="3">
+        <v>1.36557</v>
+      </c>
+      <c r="L4" s="3">
+        <f t="shared" ref="L4:L9" si="3">K$2/K4</f>
+        <v>1.0175970473868055</v>
+      </c>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+    </row>
+    <row r="5" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A5">
+        <v>4</v>
+      </c>
+      <c r="B5" s="2">
+        <v>1.2412000000000001</v>
+      </c>
+      <c r="C5" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9650499516596842</v>
+      </c>
+      <c r="D5" s="2">
+        <f t="shared" si="0"/>
+        <v>0.49126248791492105</v>
+      </c>
+      <c r="E5" s="2">
+        <f t="shared" si="1"/>
+        <v>2.5257800000000001</v>
+      </c>
+      <c r="J5">
+        <v>31</v>
+      </c>
+      <c r="K5" s="3">
+        <v>1.2412099999999999</v>
+      </c>
+      <c r="L5" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1195526945480621</v>
+      </c>
+      <c r="M5" s="2"/>
+      <c r="N5" s="2"/>
+    </row>
+    <row r="6" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A6">
+        <v>5</v>
+      </c>
+      <c r="B6" s="2">
+        <v>1.2811399999999999</v>
+      </c>
+      <c r="C6" s="2">
+        <f t="shared" si="2"/>
+        <v>1.9037888130883434</v>
+      </c>
+      <c r="D6" s="2">
+        <f t="shared" si="0"/>
+        <v>0.38075776261766869</v>
+      </c>
+      <c r="E6" s="2">
+        <f t="shared" si="1"/>
+        <v>3.9666799999999993</v>
+      </c>
+      <c r="J6">
+        <v>41</v>
+      </c>
+      <c r="K6" s="3">
+        <v>1.2907500000000001</v>
+      </c>
+      <c r="L6" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0765833817547936</v>
+      </c>
+      <c r="M6" s="2"/>
+      <c r="N6" s="2"/>
+    </row>
+    <row r="7" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" s="2">
+        <v>1.3154300000000001</v>
+      </c>
+      <c r="C7" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8541617569920101</v>
+      </c>
+      <c r="D7" s="2">
+        <f t="shared" si="0"/>
+        <v>0.30902695949866837</v>
+      </c>
+      <c r="E7" s="2">
+        <f t="shared" si="1"/>
+        <v>5.4535600000000004</v>
+      </c>
+      <c r="J7">
+        <v>51</v>
+      </c>
+      <c r="K7" s="3">
+        <v>1.22899</v>
+      </c>
+      <c r="L7" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1306845458465895</v>
+      </c>
+      <c r="M7" s="2"/>
+      <c r="N7" s="2"/>
+    </row>
+    <row r="8" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A8">
+        <v>7</v>
+      </c>
+      <c r="B8" s="2">
+        <v>1.34063</v>
+      </c>
+      <c r="C8" s="2">
+        <f t="shared" si="2"/>
+        <v>1.8193088324146112</v>
+      </c>
+      <c r="D8" s="2">
+        <f t="shared" si="0"/>
+        <v>0.25990126177351586</v>
+      </c>
+      <c r="E8" s="2">
+        <f t="shared" si="1"/>
+        <v>6.9453899999999988</v>
+      </c>
+      <c r="J8">
+        <v>61</v>
+      </c>
+      <c r="K8" s="3">
+        <v>1.2160500000000001</v>
+      </c>
+      <c r="L8" s="3">
+        <f t="shared" si="3"/>
+        <v>1.1427161712100653</v>
+      </c>
+      <c r="M8" s="2"/>
+      <c r="N8" s="2"/>
+    </row>
+    <row r="9" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="A9">
+        <v>8</v>
+      </c>
+      <c r="B9" s="2">
+        <v>1.4343300000000001</v>
+      </c>
+      <c r="C9" s="2">
+        <f t="shared" si="2"/>
+        <v>1.7004594479652522</v>
+      </c>
+      <c r="D9" s="2">
+        <f t="shared" si="0"/>
+        <v>0.21255743099565652</v>
+      </c>
+      <c r="E9" s="2">
+        <f t="shared" si="1"/>
+        <v>9.0356200000000015</v>
+      </c>
+      <c r="J9">
+        <v>71</v>
+      </c>
+      <c r="K9" s="3">
+        <v>1.28942</v>
+      </c>
+      <c r="L9" s="3">
+        <f t="shared" si="3"/>
+        <v>1.0776938468458686</v>
+      </c>
+      <c r="M9" s="2"/>
+      <c r="N9" s="2"/>
+    </row>
+    <row r="10" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J10">
+        <v>81</v>
+      </c>
+      <c r="K10" s="3">
+        <v>1.2352000000000001</v>
+      </c>
+      <c r="L10" s="3">
+        <f t="shared" ref="L10:L22" si="4">K$2/K10</f>
+        <v>1.1249999999999998</v>
+      </c>
+      <c r="M10" s="2"/>
+      <c r="N10" s="2"/>
+    </row>
+    <row r="11" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J11">
+        <v>91</v>
+      </c>
+      <c r="K11" s="3">
+        <v>1.23133</v>
+      </c>
+      <c r="L11" s="3">
+        <f t="shared" si="4"/>
+        <v>1.1285358108711718</v>
+      </c>
+      <c r="M11" s="2"/>
+      <c r="N11" s="2"/>
+    </row>
+    <row r="12" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J12">
+        <v>101</v>
+      </c>
+      <c r="K12" s="3">
+        <v>1.28267</v>
+      </c>
+      <c r="L12" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0833651679699376</v>
+      </c>
+      <c r="M12" s="2"/>
+      <c r="N12" s="2"/>
+    </row>
+    <row r="13" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J13">
+        <v>111</v>
+      </c>
+      <c r="K13" s="3">
+        <v>1.3347800000000001</v>
+      </c>
+      <c r="L13" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0410704385741469</v>
+      </c>
+      <c r="M13" s="2"/>
+      <c r="N13" s="2"/>
+    </row>
+    <row r="14" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J14">
+        <v>121</v>
+      </c>
+      <c r="K14" s="3">
+        <v>1.2574399999999999</v>
+      </c>
+      <c r="L14" s="3">
+        <f t="shared" si="4"/>
+        <v>1.1051024303346482</v>
+      </c>
+      <c r="M14" s="2"/>
+      <c r="N14" s="2"/>
+    </row>
+    <row r="15" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J15">
+        <v>131</v>
+      </c>
+      <c r="K15" s="3">
+        <v>1.2799799999999999</v>
+      </c>
+      <c r="L15" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0856419631556744</v>
+      </c>
+      <c r="M15" s="2"/>
+      <c r="N15" s="2"/>
+    </row>
+    <row r="16" spans="1:14" x14ac:dyDescent="0.3">
+      <c r="J16">
+        <v>141</v>
+      </c>
+      <c r="K16" s="3">
+        <v>1.44651</v>
+      </c>
+      <c r="L16" s="3">
+        <f t="shared" si="4"/>
+        <v>0.96065702967832922</v>
+      </c>
+      <c r="M16" s="2"/>
+      <c r="N16" s="2"/>
+    </row>
+    <row r="17" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J17">
+        <v>151</v>
+      </c>
+      <c r="K17" s="3">
+        <v>1.4887900000000001</v>
+      </c>
+      <c r="L17" s="3">
+        <f t="shared" si="4"/>
+        <v>0.93337542568125786</v>
+      </c>
+      <c r="M17" s="2"/>
+      <c r="N17" s="2"/>
+    </row>
+    <row r="18" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J18">
+        <v>161</v>
+      </c>
+      <c r="K18" s="3">
+        <v>1.3243</v>
+      </c>
+      <c r="L18" s="3">
+        <f t="shared" si="4"/>
+        <v>1.0493090689420825</v>
+      </c>
+      <c r="M18" s="2"/>
+      <c r="N18" s="2"/>
+    </row>
+    <row r="19" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J19">
+        <v>171</v>
+      </c>
+      <c r="K19" s="3">
+        <v>1.34728</v>
+      </c>
+      <c r="L19" s="3">
+        <f t="shared" si="4"/>
+        <v>1.031411436375512</v>
+      </c>
+      <c r="M19" s="2"/>
+      <c r="N19" s="2"/>
+    </row>
+    <row r="20" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J20">
+        <v>181</v>
+      </c>
+      <c r="K20" s="3">
+        <v>1.35225</v>
+      </c>
+      <c r="L20" s="3">
+        <f t="shared" si="4"/>
+        <v>1.027620632279534</v>
+      </c>
+      <c r="M20" s="2"/>
+      <c r="N20" s="2"/>
+    </row>
+    <row r="21" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J21">
+        <v>191</v>
+      </c>
+      <c r="K21" s="3">
+        <v>1.43207</v>
+      </c>
+      <c r="L21" s="3">
+        <f t="shared" si="4"/>
+        <v>0.97034362845391631</v>
+      </c>
+      <c r="M21" s="2"/>
+      <c r="N21" s="2"/>
+    </row>
+    <row r="22" spans="10:14" x14ac:dyDescent="0.3">
+      <c r="J22">
+        <v>201</v>
+      </c>
+      <c r="K22" s="3">
+        <v>1.40455</v>
+      </c>
+      <c r="L22" s="3">
+        <f t="shared" si="4"/>
+        <v>0.98935602150154855</v>
+      </c>
+      <c r="M22" s="2"/>
+      <c r="N22" s="2"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{42EF08DA-F069-4231-BB45-B0F7DB12E3BB}">
   <dimension ref="A1:F161"/>
   <sheetViews>
@@ -11465,12 +14731,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{14EB68CC-BDD0-4E94-80EA-24CBDB8BF46B}">
   <dimension ref="A1:H160"/>
   <sheetViews>
     <sheetView zoomScale="97" workbookViewId="0">
-      <selection activeCell="L23" sqref="L23"/>
+      <selection activeCell="I8" sqref="I8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -14684,11 +17950,11 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2A99950E-ECAB-4AD6-82DA-4358D4663E12}">
   <dimension ref="A1:E161"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+    <sheetView topLeftCell="B1" workbookViewId="0">
       <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
@@ -16625,7 +19891,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{24D04B6D-C203-4DA7-98F9-CEDA1ABD8977}">
   <dimension ref="A1:H48"/>
   <sheetViews>

</xml_diff>